<commit_message>
scooter.csv innehåller nu alla scootrar, 1 skövde 2 lund 3 uppsala
</commit_message>
<xml_diff>
--- a/sql-scripts/scooter_skovde.xlsx
+++ b/sql-scripts/scooter_skovde.xlsx
@@ -378,7 +378,7 @@
   <dimension ref="A1:I1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H2" sqref="H2:H335"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -434,7 +434,7 @@
       <c r="G2" s="1">
         <v>0</v>
       </c>
-      <c r="H2" s="1">
+      <c r="H2">
         <v>68</v>
       </c>
       <c r="I2" s="1" t="s">
@@ -463,7 +463,7 @@
       <c r="G3" s="1">
         <v>0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="H3">
         <v>76</v>
       </c>
       <c r="I3" s="1" t="s">
@@ -492,7 +492,7 @@
       <c r="G4" s="1">
         <v>0</v>
       </c>
-      <c r="H4" s="1">
+      <c r="H4">
         <v>36</v>
       </c>
       <c r="I4" s="1" t="s">
@@ -521,7 +521,7 @@
       <c r="G5" s="1">
         <v>0</v>
       </c>
-      <c r="H5" s="1">
+      <c r="H5">
         <v>31</v>
       </c>
       <c r="I5" s="1" t="s">
@@ -550,7 +550,7 @@
       <c r="G6" s="1">
         <v>0</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6">
         <v>55</v>
       </c>
       <c r="I6" s="1" t="s">
@@ -579,7 +579,7 @@
       <c r="G7" s="1">
         <v>0</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7">
         <v>39</v>
       </c>
       <c r="I7" s="1" t="s">
@@ -608,7 +608,7 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8">
         <v>25</v>
       </c>
       <c r="I8" s="1" t="s">
@@ -637,7 +637,7 @@
       <c r="G9" s="1">
         <v>0</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9">
         <v>60</v>
       </c>
       <c r="I9" s="1" t="s">
@@ -666,7 +666,7 @@
       <c r="G10" s="1">
         <v>0</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10">
         <v>51</v>
       </c>
       <c r="I10" s="1" t="s">
@@ -695,7 +695,7 @@
       <c r="G11" s="1">
         <v>0</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11">
         <v>82</v>
       </c>
       <c r="I11" s="1" t="s">
@@ -724,7 +724,7 @@
       <c r="G12" s="1">
         <v>0</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12">
         <v>28</v>
       </c>
       <c r="I12" s="1" t="s">
@@ -753,7 +753,7 @@
       <c r="G13" s="1">
         <v>0</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13">
         <v>20</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -782,7 +782,7 @@
       <c r="G14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14">
         <v>86</v>
       </c>
       <c r="I14" s="1" t="s">
@@ -811,8 +811,8 @@
       <c r="G15" s="1">
         <v>0</v>
       </c>
-      <c r="H15" s="1">
-        <v>3</v>
+      <c r="H15">
+        <v>15</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>6</v>
@@ -840,7 +840,7 @@
       <c r="G16" s="1">
         <v>0</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16">
         <v>14</v>
       </c>
       <c r="I16" s="1" t="s">
@@ -869,7 +869,7 @@
       <c r="G17" s="1">
         <v>0</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17">
         <v>28</v>
       </c>
       <c r="I17" s="1" t="s">
@@ -898,8 +898,8 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-      <c r="H18" s="1">
-        <v>1</v>
+      <c r="H18">
+        <v>77</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>6</v>
@@ -927,8 +927,8 @@
       <c r="G19" s="1">
         <v>0</v>
       </c>
-      <c r="H19" s="1">
-        <v>4</v>
+      <c r="H19">
+        <v>43</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>6</v>
@@ -956,7 +956,7 @@
       <c r="G20" s="1">
         <v>0</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20">
         <v>10</v>
       </c>
       <c r="I20" s="1" t="s">
@@ -985,7 +985,7 @@
       <c r="G21" s="1">
         <v>0</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21">
         <v>76</v>
       </c>
       <c r="I21" s="1" t="s">
@@ -1014,7 +1014,7 @@
       <c r="G22" s="1">
         <v>0</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22">
         <v>91</v>
       </c>
       <c r="I22" s="1" t="s">
@@ -1043,7 +1043,7 @@
       <c r="G23" s="1">
         <v>0</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23">
         <v>63</v>
       </c>
       <c r="I23" s="1" t="s">
@@ -1072,7 +1072,7 @@
       <c r="G24" s="1">
         <v>0</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24">
         <v>91</v>
       </c>
       <c r="I24" s="1" t="s">
@@ -1101,7 +1101,7 @@
       <c r="G25" s="1">
         <v>0</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25">
         <v>29</v>
       </c>
       <c r="I25" s="1" t="s">
@@ -1130,7 +1130,7 @@
       <c r="G26" s="1">
         <v>0</v>
       </c>
-      <c r="H26" s="1">
+      <c r="H26">
         <v>87</v>
       </c>
       <c r="I26" s="1" t="s">
@@ -1159,7 +1159,7 @@
       <c r="G27" s="1">
         <v>0</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H27">
         <v>94</v>
       </c>
       <c r="I27" s="1" t="s">
@@ -1188,7 +1188,7 @@
       <c r="G28" s="1">
         <v>0</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H28">
         <v>78</v>
       </c>
       <c r="I28" s="1" t="s">
@@ -1217,7 +1217,7 @@
       <c r="G29" s="1">
         <v>0</v>
       </c>
-      <c r="H29" s="1">
+      <c r="H29">
         <v>41</v>
       </c>
       <c r="I29" s="1" t="s">
@@ -1246,7 +1246,7 @@
       <c r="G30" s="1">
         <v>0</v>
       </c>
-      <c r="H30" s="1">
+      <c r="H30">
         <v>96</v>
       </c>
       <c r="I30" s="1" t="s">
@@ -1275,7 +1275,7 @@
       <c r="G31" s="1">
         <v>0</v>
       </c>
-      <c r="H31" s="1">
+      <c r="H31">
         <v>53</v>
       </c>
       <c r="I31" s="1" t="s">
@@ -1304,7 +1304,7 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="1">
+      <c r="H32">
         <v>19</v>
       </c>
       <c r="I32" s="1" t="s">
@@ -1333,7 +1333,7 @@
       <c r="G33" s="1">
         <v>0</v>
       </c>
-      <c r="H33" s="1">
+      <c r="H33">
         <v>80</v>
       </c>
       <c r="I33" s="1" t="s">
@@ -1362,7 +1362,7 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="1">
+      <c r="H34">
         <v>50</v>
       </c>
       <c r="I34" s="1" t="s">
@@ -1391,8 +1391,8 @@
       <c r="G35" s="1">
         <v>0</v>
       </c>
-      <c r="H35" s="1">
-        <v>0</v>
+      <c r="H35">
+        <v>18</v>
       </c>
       <c r="I35" s="1" t="s">
         <v>6</v>
@@ -1420,7 +1420,7 @@
       <c r="G36" s="1">
         <v>0</v>
       </c>
-      <c r="H36" s="1">
+      <c r="H36">
         <v>25</v>
       </c>
       <c r="I36" s="1" t="s">
@@ -1449,7 +1449,7 @@
       <c r="G37" s="1">
         <v>0</v>
       </c>
-      <c r="H37" s="1">
+      <c r="H37">
         <v>80</v>
       </c>
       <c r="I37" s="1" t="s">
@@ -1478,7 +1478,7 @@
       <c r="G38" s="1">
         <v>0</v>
       </c>
-      <c r="H38" s="1">
+      <c r="H38">
         <v>24</v>
       </c>
       <c r="I38" s="1" t="s">
@@ -1507,7 +1507,7 @@
       <c r="G39" s="1">
         <v>0</v>
       </c>
-      <c r="H39" s="1">
+      <c r="H39">
         <v>16</v>
       </c>
       <c r="I39" s="1" t="s">
@@ -1536,8 +1536,8 @@
       <c r="G40" s="1">
         <v>0</v>
       </c>
-      <c r="H40" s="1">
-        <v>2</v>
+      <c r="H40">
+        <v>20</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>6</v>
@@ -1565,7 +1565,7 @@
       <c r="G41" s="1">
         <v>0</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H41">
         <v>13</v>
       </c>
       <c r="I41" s="1" t="s">
@@ -1594,7 +1594,7 @@
       <c r="G42" s="1">
         <v>0</v>
       </c>
-      <c r="H42" s="1">
+      <c r="H42">
         <v>96</v>
       </c>
       <c r="I42" s="1" t="s">
@@ -1623,8 +1623,8 @@
       <c r="G43" s="1">
         <v>0</v>
       </c>
-      <c r="H43" s="1">
-        <v>0</v>
+      <c r="H43">
+        <v>44</v>
       </c>
       <c r="I43" s="1" t="s">
         <v>6</v>
@@ -1652,7 +1652,7 @@
       <c r="G44" s="1">
         <v>0</v>
       </c>
-      <c r="H44" s="1">
+      <c r="H44">
         <v>36</v>
       </c>
       <c r="I44" s="1" t="s">
@@ -1681,7 +1681,7 @@
       <c r="G45" s="1">
         <v>0</v>
       </c>
-      <c r="H45" s="1">
+      <c r="H45">
         <v>46</v>
       </c>
       <c r="I45" s="1" t="s">
@@ -1710,7 +1710,7 @@
       <c r="G46" s="1">
         <v>0</v>
       </c>
-      <c r="H46" s="1">
+      <c r="H46">
         <v>39</v>
       </c>
       <c r="I46" s="1" t="s">
@@ -1739,7 +1739,7 @@
       <c r="G47" s="1">
         <v>0</v>
       </c>
-      <c r="H47" s="1">
+      <c r="H47">
         <v>85</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -1768,7 +1768,7 @@
       <c r="G48" s="1">
         <v>0</v>
       </c>
-      <c r="H48" s="1">
+      <c r="H48">
         <v>89</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -1797,7 +1797,7 @@
       <c r="G49" s="1">
         <v>0</v>
       </c>
-      <c r="H49" s="1">
+      <c r="H49">
         <v>76</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -1826,7 +1826,7 @@
       <c r="G50" s="1">
         <v>0</v>
       </c>
-      <c r="H50" s="1">
+      <c r="H50">
         <v>17</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -1855,7 +1855,7 @@
       <c r="G51" s="1">
         <v>0</v>
       </c>
-      <c r="H51" s="1">
+      <c r="H51">
         <v>86</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -1884,7 +1884,7 @@
       <c r="G52" s="1">
         <v>0</v>
       </c>
-      <c r="H52" s="1">
+      <c r="H52">
         <v>24</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -1913,7 +1913,7 @@
       <c r="G53" s="1">
         <v>0</v>
       </c>
-      <c r="H53" s="1">
+      <c r="H53">
         <v>96</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -1942,7 +1942,7 @@
       <c r="G54" s="1">
         <v>0</v>
       </c>
-      <c r="H54" s="1">
+      <c r="H54">
         <v>83</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -1971,7 +1971,7 @@
       <c r="G55" s="1">
         <v>0</v>
       </c>
-      <c r="H55" s="1">
+      <c r="H55">
         <v>18</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -2000,8 +2000,8 @@
       <c r="G56" s="1">
         <v>0</v>
       </c>
-      <c r="H56" s="1">
-        <v>7</v>
+      <c r="H56">
+        <v>62</v>
       </c>
       <c r="I56" s="1" t="s">
         <v>6</v>
@@ -2029,7 +2029,7 @@
       <c r="G57" s="1">
         <v>0</v>
       </c>
-      <c r="H57" s="1">
+      <c r="H57">
         <v>93</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -2058,7 +2058,7 @@
       <c r="G58" s="1">
         <v>0</v>
       </c>
-      <c r="H58" s="1">
+      <c r="H58">
         <v>12</v>
       </c>
       <c r="I58" s="1" t="s">
@@ -2087,7 +2087,7 @@
       <c r="G59" s="1">
         <v>0</v>
       </c>
-      <c r="H59" s="1">
+      <c r="H59">
         <v>26</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -2116,7 +2116,7 @@
       <c r="G60" s="1">
         <v>0</v>
       </c>
-      <c r="H60" s="1">
+      <c r="H60">
         <v>84</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -2145,7 +2145,7 @@
       <c r="G61" s="1">
         <v>0</v>
       </c>
-      <c r="H61" s="1">
+      <c r="H61">
         <v>52</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -2174,7 +2174,7 @@
       <c r="G62" s="1">
         <v>0</v>
       </c>
-      <c r="H62" s="1">
+      <c r="H62">
         <v>77</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -2203,7 +2203,7 @@
       <c r="G63" s="1">
         <v>0</v>
       </c>
-      <c r="H63" s="1">
+      <c r="H63">
         <v>58</v>
       </c>
       <c r="I63" s="1" t="s">
@@ -2232,7 +2232,7 @@
       <c r="G64" s="1">
         <v>0</v>
       </c>
-      <c r="H64" s="1">
+      <c r="H64">
         <v>41</v>
       </c>
       <c r="I64" s="1" t="s">
@@ -2261,7 +2261,7 @@
       <c r="G65" s="1">
         <v>0</v>
       </c>
-      <c r="H65" s="1">
+      <c r="H65">
         <v>63</v>
       </c>
       <c r="I65" s="1" t="s">
@@ -2290,7 +2290,7 @@
       <c r="G66" s="1">
         <v>0</v>
       </c>
-      <c r="H66" s="1">
+      <c r="H66">
         <v>20</v>
       </c>
       <c r="I66" s="1" t="s">
@@ -2319,7 +2319,7 @@
       <c r="G67" s="1">
         <v>0</v>
       </c>
-      <c r="H67" s="1">
+      <c r="H67">
         <v>25</v>
       </c>
       <c r="I67" s="1" t="s">
@@ -2348,7 +2348,7 @@
       <c r="G68" s="1">
         <v>0</v>
       </c>
-      <c r="H68" s="1">
+      <c r="H68">
         <v>99</v>
       </c>
       <c r="I68" s="1" t="s">
@@ -2377,7 +2377,7 @@
       <c r="G69" s="1">
         <v>0</v>
       </c>
-      <c r="H69" s="1">
+      <c r="H69">
         <v>100</v>
       </c>
       <c r="I69" s="1" t="s">
@@ -2406,7 +2406,7 @@
       <c r="G70" s="1">
         <v>0</v>
       </c>
-      <c r="H70" s="1">
+      <c r="H70">
         <v>82</v>
       </c>
       <c r="I70" s="1" t="s">
@@ -2435,7 +2435,7 @@
       <c r="G71" s="1">
         <v>0</v>
       </c>
-      <c r="H71" s="1">
+      <c r="H71">
         <v>12</v>
       </c>
       <c r="I71" s="1" t="s">
@@ -2464,7 +2464,7 @@
       <c r="G72" s="1">
         <v>0</v>
       </c>
-      <c r="H72" s="1">
+      <c r="H72">
         <v>15</v>
       </c>
       <c r="I72" s="1" t="s">
@@ -2493,7 +2493,7 @@
       <c r="G73" s="1">
         <v>0</v>
       </c>
-      <c r="H73" s="1">
+      <c r="H73">
         <v>75</v>
       </c>
       <c r="I73" s="1" t="s">
@@ -2522,7 +2522,7 @@
       <c r="G74" s="1">
         <v>0</v>
       </c>
-      <c r="H74" s="1">
+      <c r="H74">
         <v>88</v>
       </c>
       <c r="I74" s="1" t="s">
@@ -2551,7 +2551,7 @@
       <c r="G75" s="1">
         <v>0</v>
       </c>
-      <c r="H75" s="1">
+      <c r="H75">
         <v>91</v>
       </c>
       <c r="I75" s="1" t="s">
@@ -2580,7 +2580,7 @@
       <c r="G76" s="1">
         <v>0</v>
       </c>
-      <c r="H76" s="1">
+      <c r="H76">
         <v>43</v>
       </c>
       <c r="I76" s="1" t="s">
@@ -2609,7 +2609,7 @@
       <c r="G77" s="1">
         <v>0</v>
       </c>
-      <c r="H77" s="1">
+      <c r="H77">
         <v>88</v>
       </c>
       <c r="I77" s="1" t="s">
@@ -2638,7 +2638,7 @@
       <c r="G78" s="1">
         <v>0</v>
       </c>
-      <c r="H78" s="1">
+      <c r="H78">
         <v>97</v>
       </c>
       <c r="I78" s="1" t="s">
@@ -2667,7 +2667,7 @@
       <c r="G79" s="1">
         <v>0</v>
       </c>
-      <c r="H79" s="1">
+      <c r="H79">
         <v>27</v>
       </c>
       <c r="I79" s="1" t="s">
@@ -2696,7 +2696,7 @@
       <c r="G80" s="1">
         <v>0</v>
       </c>
-      <c r="H80" s="1">
+      <c r="H80">
         <v>61</v>
       </c>
       <c r="I80" s="1" t="s">
@@ -2725,7 +2725,7 @@
       <c r="G81" s="1">
         <v>0</v>
       </c>
-      <c r="H81" s="1">
+      <c r="H81">
         <v>17</v>
       </c>
       <c r="I81" s="1" t="s">
@@ -2754,7 +2754,7 @@
       <c r="G82" s="1">
         <v>0</v>
       </c>
-      <c r="H82" s="1">
+      <c r="H82">
         <v>26</v>
       </c>
       <c r="I82" s="1" t="s">
@@ -2783,7 +2783,7 @@
       <c r="G83" s="1">
         <v>0</v>
       </c>
-      <c r="H83" s="1">
+      <c r="H83">
         <v>34</v>
       </c>
       <c r="I83" s="1" t="s">
@@ -2812,7 +2812,7 @@
       <c r="G84" s="1">
         <v>0</v>
       </c>
-      <c r="H84" s="1">
+      <c r="H84">
         <v>100</v>
       </c>
       <c r="I84" s="1" t="s">
@@ -2841,7 +2841,7 @@
       <c r="G85" s="1">
         <v>0</v>
       </c>
-      <c r="H85" s="1">
+      <c r="H85">
         <v>83</v>
       </c>
       <c r="I85" s="1" t="s">
@@ -2870,7 +2870,7 @@
       <c r="G86" s="1">
         <v>0</v>
       </c>
-      <c r="H86" s="1">
+      <c r="H86">
         <v>95</v>
       </c>
       <c r="I86" s="1" t="s">
@@ -2899,7 +2899,7 @@
       <c r="G87" s="1">
         <v>0</v>
       </c>
-      <c r="H87" s="1">
+      <c r="H87">
         <v>29</v>
       </c>
       <c r="I87" s="1" t="s">
@@ -2928,7 +2928,7 @@
       <c r="G88" s="1">
         <v>0</v>
       </c>
-      <c r="H88" s="1">
+      <c r="H88">
         <v>37</v>
       </c>
       <c r="I88" s="1" t="s">
@@ -2957,7 +2957,7 @@
       <c r="G89" s="1">
         <v>0</v>
       </c>
-      <c r="H89" s="1">
+      <c r="H89">
         <v>62</v>
       </c>
       <c r="I89" s="1" t="s">
@@ -2986,7 +2986,7 @@
       <c r="G90" s="1">
         <v>0</v>
       </c>
-      <c r="H90" s="1">
+      <c r="H90">
         <v>34</v>
       </c>
       <c r="I90" s="1" t="s">
@@ -3015,7 +3015,7 @@
       <c r="G91" s="1">
         <v>0</v>
       </c>
-      <c r="H91" s="1">
+      <c r="H91">
         <v>19</v>
       </c>
       <c r="I91" s="1" t="s">
@@ -3044,7 +3044,7 @@
       <c r="G92" s="1">
         <v>0</v>
       </c>
-      <c r="H92" s="1">
+      <c r="H92">
         <v>100</v>
       </c>
       <c r="I92" s="1" t="s">
@@ -3073,7 +3073,7 @@
       <c r="G93" s="1">
         <v>0</v>
       </c>
-      <c r="H93" s="1">
+      <c r="H93">
         <v>98</v>
       </c>
       <c r="I93" s="1" t="s">
@@ -3102,7 +3102,7 @@
       <c r="G94" s="1">
         <v>0</v>
       </c>
-      <c r="H94" s="1">
+      <c r="H94">
         <v>16</v>
       </c>
       <c r="I94" s="1" t="s">
@@ -3131,7 +3131,7 @@
       <c r="G95" s="1">
         <v>0</v>
       </c>
-      <c r="H95" s="1">
+      <c r="H95">
         <v>29</v>
       </c>
       <c r="I95" s="1" t="s">
@@ -3160,7 +3160,7 @@
       <c r="G96" s="1">
         <v>0</v>
       </c>
-      <c r="H96" s="1">
+      <c r="H96">
         <v>54</v>
       </c>
       <c r="I96" s="1" t="s">
@@ -3189,7 +3189,7 @@
       <c r="G97" s="1">
         <v>0</v>
       </c>
-      <c r="H97" s="1">
+      <c r="H97">
         <v>51</v>
       </c>
       <c r="I97" s="1" t="s">
@@ -3218,7 +3218,7 @@
       <c r="G98" s="1">
         <v>0</v>
       </c>
-      <c r="H98" s="1">
+      <c r="H98">
         <v>50</v>
       </c>
       <c r="I98" s="1" t="s">
@@ -3247,7 +3247,7 @@
       <c r="G99" s="1">
         <v>0</v>
       </c>
-      <c r="H99" s="1">
+      <c r="H99">
         <v>63</v>
       </c>
       <c r="I99" s="1" t="s">
@@ -3276,7 +3276,7 @@
       <c r="G100" s="1">
         <v>0</v>
       </c>
-      <c r="H100" s="1">
+      <c r="H100">
         <v>65</v>
       </c>
       <c r="I100" s="1" t="s">
@@ -3305,7 +3305,7 @@
       <c r="G101" s="1">
         <v>0</v>
       </c>
-      <c r="H101" s="1">
+      <c r="H101">
         <v>78</v>
       </c>
       <c r="I101" s="1" t="s">
@@ -3334,8 +3334,8 @@
       <c r="G102" s="1">
         <v>0</v>
       </c>
-      <c r="H102" s="1">
-        <v>5</v>
+      <c r="H102">
+        <v>55</v>
       </c>
       <c r="I102" s="1" t="s">
         <v>6</v>
@@ -3363,7 +3363,7 @@
       <c r="G103" s="1">
         <v>0</v>
       </c>
-      <c r="H103" s="1">
+      <c r="H103">
         <v>34</v>
       </c>
       <c r="I103" s="1" t="s">
@@ -3392,7 +3392,7 @@
       <c r="G104" s="1">
         <v>0</v>
       </c>
-      <c r="H104" s="1">
+      <c r="H104">
         <v>27</v>
       </c>
       <c r="I104" s="1" t="s">
@@ -3421,7 +3421,7 @@
       <c r="G105" s="1">
         <v>0</v>
       </c>
-      <c r="H105" s="1">
+      <c r="H105">
         <v>69</v>
       </c>
       <c r="I105" s="1" t="s">
@@ -3450,7 +3450,7 @@
       <c r="G106" s="1">
         <v>0</v>
       </c>
-      <c r="H106" s="1">
+      <c r="H106">
         <v>42</v>
       </c>
       <c r="I106" s="1" t="s">
@@ -3479,7 +3479,7 @@
       <c r="G107" s="1">
         <v>0</v>
       </c>
-      <c r="H107" s="1">
+      <c r="H107">
         <v>18</v>
       </c>
       <c r="I107" s="1" t="s">
@@ -3508,8 +3508,8 @@
       <c r="G108" s="1">
         <v>0</v>
       </c>
-      <c r="H108" s="1">
-        <v>4</v>
+      <c r="H108">
+        <v>30</v>
       </c>
       <c r="I108" s="1" t="s">
         <v>6</v>
@@ -3537,7 +3537,7 @@
       <c r="G109" s="1">
         <v>0</v>
       </c>
-      <c r="H109" s="1">
+      <c r="H109">
         <v>91</v>
       </c>
       <c r="I109" s="1" t="s">
@@ -3566,7 +3566,7 @@
       <c r="G110" s="1">
         <v>0</v>
       </c>
-      <c r="H110" s="1">
+      <c r="H110">
         <v>90</v>
       </c>
       <c r="I110" s="1" t="s">
@@ -3595,7 +3595,7 @@
       <c r="G111" s="1">
         <v>0</v>
       </c>
-      <c r="H111" s="1">
+      <c r="H111">
         <v>84</v>
       </c>
       <c r="I111" s="1" t="s">
@@ -3624,7 +3624,7 @@
       <c r="G112" s="1">
         <v>0</v>
       </c>
-      <c r="H112" s="1">
+      <c r="H112">
         <v>24</v>
       </c>
       <c r="I112" s="1" t="s">
@@ -3653,7 +3653,7 @@
       <c r="G113" s="1">
         <v>0</v>
       </c>
-      <c r="H113" s="1">
+      <c r="H113">
         <v>21</v>
       </c>
       <c r="I113" s="1" t="s">
@@ -3682,7 +3682,7 @@
       <c r="G114" s="1">
         <v>0</v>
       </c>
-      <c r="H114" s="1">
+      <c r="H114">
         <v>43</v>
       </c>
       <c r="I114" s="1" t="s">
@@ -3711,7 +3711,7 @@
       <c r="G115" s="1">
         <v>0</v>
       </c>
-      <c r="H115" s="1">
+      <c r="H115">
         <v>14</v>
       </c>
       <c r="I115" s="1" t="s">
@@ -3740,7 +3740,7 @@
       <c r="G116" s="1">
         <v>0</v>
       </c>
-      <c r="H116" s="1">
+      <c r="H116">
         <v>90</v>
       </c>
       <c r="I116" s="1" t="s">
@@ -3769,7 +3769,7 @@
       <c r="G117" s="1">
         <v>0</v>
       </c>
-      <c r="H117" s="1">
+      <c r="H117">
         <v>12</v>
       </c>
       <c r="I117" s="1" t="s">
@@ -3798,7 +3798,7 @@
       <c r="G118" s="1">
         <v>0</v>
       </c>
-      <c r="H118" s="1">
+      <c r="H118">
         <v>68</v>
       </c>
       <c r="I118" s="1" t="s">
@@ -3827,7 +3827,7 @@
       <c r="G119" s="1">
         <v>0</v>
       </c>
-      <c r="H119" s="1">
+      <c r="H119">
         <v>97</v>
       </c>
       <c r="I119" s="1" t="s">
@@ -3856,7 +3856,7 @@
       <c r="G120" s="1">
         <v>0</v>
       </c>
-      <c r="H120" s="1">
+      <c r="H120">
         <v>91</v>
       </c>
       <c r="I120" s="1" t="s">
@@ -3885,7 +3885,7 @@
       <c r="G121" s="1">
         <v>0</v>
       </c>
-      <c r="H121" s="1">
+      <c r="H121">
         <v>67</v>
       </c>
       <c r="I121" s="1" t="s">
@@ -3914,7 +3914,7 @@
       <c r="G122" s="1">
         <v>0</v>
       </c>
-      <c r="H122" s="1">
+      <c r="H122">
         <v>16</v>
       </c>
       <c r="I122" s="1" t="s">
@@ -3943,7 +3943,7 @@
       <c r="G123" s="1">
         <v>0</v>
       </c>
-      <c r="H123" s="1">
+      <c r="H123">
         <v>23</v>
       </c>
       <c r="I123" s="1" t="s">
@@ -3972,7 +3972,7 @@
       <c r="G124" s="1">
         <v>0</v>
       </c>
-      <c r="H124" s="1">
+      <c r="H124">
         <v>11</v>
       </c>
       <c r="I124" s="1" t="s">
@@ -4001,7 +4001,7 @@
       <c r="G125" s="1">
         <v>0</v>
       </c>
-      <c r="H125" s="1">
+      <c r="H125">
         <v>42</v>
       </c>
       <c r="I125" s="1" t="s">
@@ -4030,7 +4030,7 @@
       <c r="G126" s="1">
         <v>0</v>
       </c>
-      <c r="H126" s="1">
+      <c r="H126">
         <v>87</v>
       </c>
       <c r="I126" s="1" t="s">
@@ -4059,7 +4059,7 @@
       <c r="G127" s="1">
         <v>0</v>
       </c>
-      <c r="H127" s="1">
+      <c r="H127">
         <v>90</v>
       </c>
       <c r="I127" s="1" t="s">
@@ -4088,7 +4088,7 @@
       <c r="G128" s="1">
         <v>0</v>
       </c>
-      <c r="H128" s="1">
+      <c r="H128">
         <v>29</v>
       </c>
       <c r="I128" s="1" t="s">
@@ -4117,7 +4117,7 @@
       <c r="G129" s="1">
         <v>0</v>
       </c>
-      <c r="H129" s="1">
+      <c r="H129">
         <v>96</v>
       </c>
       <c r="I129" s="1" t="s">
@@ -4146,7 +4146,7 @@
       <c r="G130" s="1">
         <v>0</v>
       </c>
-      <c r="H130" s="1">
+      <c r="H130">
         <v>69</v>
       </c>
       <c r="I130" s="1" t="s">
@@ -4175,7 +4175,7 @@
       <c r="G131" s="1">
         <v>0</v>
       </c>
-      <c r="H131" s="1">
+      <c r="H131">
         <v>80</v>
       </c>
       <c r="I131" s="1" t="s">
@@ -4204,7 +4204,7 @@
       <c r="G132" s="1">
         <v>0</v>
       </c>
-      <c r="H132" s="1">
+      <c r="H132">
         <v>56</v>
       </c>
       <c r="I132" s="1" t="s">
@@ -4233,7 +4233,7 @@
       <c r="G133" s="1">
         <v>0</v>
       </c>
-      <c r="H133" s="1">
+      <c r="H133">
         <v>30</v>
       </c>
       <c r="I133" s="1" t="s">
@@ -4262,8 +4262,8 @@
       <c r="G134" s="1">
         <v>0</v>
       </c>
-      <c r="H134" s="1">
-        <v>9</v>
+      <c r="H134">
+        <v>11</v>
       </c>
       <c r="I134" s="1" t="s">
         <v>6</v>
@@ -4291,7 +4291,7 @@
       <c r="G135" s="1">
         <v>0</v>
       </c>
-      <c r="H135" s="1">
+      <c r="H135">
         <v>16</v>
       </c>
       <c r="I135" s="1" t="s">
@@ -4320,7 +4320,7 @@
       <c r="G136" s="1">
         <v>0</v>
       </c>
-      <c r="H136" s="1">
+      <c r="H136">
         <v>15</v>
       </c>
       <c r="I136" s="1" t="s">
@@ -4349,7 +4349,7 @@
       <c r="G137" s="1">
         <v>0</v>
       </c>
-      <c r="H137" s="1">
+      <c r="H137">
         <v>95</v>
       </c>
       <c r="I137" s="1" t="s">
@@ -4378,7 +4378,7 @@
       <c r="G138" s="1">
         <v>0</v>
       </c>
-      <c r="H138" s="1">
+      <c r="H138">
         <v>24</v>
       </c>
       <c r="I138" s="1" t="s">
@@ -4407,7 +4407,7 @@
       <c r="G139" s="1">
         <v>0</v>
       </c>
-      <c r="H139" s="1">
+      <c r="H139">
         <v>51</v>
       </c>
       <c r="I139" s="1" t="s">
@@ -4436,7 +4436,7 @@
       <c r="G140" s="1">
         <v>0</v>
       </c>
-      <c r="H140" s="1">
+      <c r="H140">
         <v>24</v>
       </c>
       <c r="I140" s="1" t="s">
@@ -4465,7 +4465,7 @@
       <c r="G141" s="1">
         <v>0</v>
       </c>
-      <c r="H141" s="1">
+      <c r="H141">
         <v>41</v>
       </c>
       <c r="I141" s="1" t="s">
@@ -4494,7 +4494,7 @@
       <c r="G142" s="1">
         <v>0</v>
       </c>
-      <c r="H142" s="1">
+      <c r="H142">
         <v>22</v>
       </c>
       <c r="I142" s="1" t="s">
@@ -4523,7 +4523,7 @@
       <c r="G143" s="1">
         <v>0</v>
       </c>
-      <c r="H143" s="1">
+      <c r="H143">
         <v>97</v>
       </c>
       <c r="I143" s="1" t="s">
@@ -4552,7 +4552,7 @@
       <c r="G144" s="1">
         <v>0</v>
       </c>
-      <c r="H144" s="1">
+      <c r="H144">
         <v>10</v>
       </c>
       <c r="I144" s="1" t="s">
@@ -4581,7 +4581,7 @@
       <c r="G145" s="1">
         <v>0</v>
       </c>
-      <c r="H145" s="1">
+      <c r="H145">
         <v>71</v>
       </c>
       <c r="I145" s="1" t="s">
@@ -4610,7 +4610,7 @@
       <c r="G146" s="1">
         <v>0</v>
       </c>
-      <c r="H146" s="1">
+      <c r="H146">
         <v>88</v>
       </c>
       <c r="I146" s="1" t="s">
@@ -4639,7 +4639,7 @@
       <c r="G147" s="1">
         <v>0</v>
       </c>
-      <c r="H147" s="1">
+      <c r="H147">
         <v>98</v>
       </c>
       <c r="I147" s="1" t="s">
@@ -4668,7 +4668,7 @@
       <c r="G148" s="1">
         <v>0</v>
       </c>
-      <c r="H148" s="1">
+      <c r="H148">
         <v>81</v>
       </c>
       <c r="I148" s="1" t="s">
@@ -4697,8 +4697,8 @@
       <c r="G149" s="1">
         <v>0</v>
       </c>
-      <c r="H149" s="1">
-        <v>2</v>
+      <c r="H149">
+        <v>49</v>
       </c>
       <c r="I149" s="1" t="s">
         <v>6</v>
@@ -4726,7 +4726,7 @@
       <c r="G150" s="1">
         <v>0</v>
       </c>
-      <c r="H150" s="1">
+      <c r="H150">
         <v>56</v>
       </c>
       <c r="I150" s="1" t="s">
@@ -4755,8 +4755,8 @@
       <c r="G151" s="1">
         <v>0</v>
       </c>
-      <c r="H151" s="1">
-        <v>9</v>
+      <c r="H151">
+        <v>72</v>
       </c>
       <c r="I151" s="1" t="s">
         <v>6</v>
@@ -4784,7 +4784,7 @@
       <c r="G152" s="1">
         <v>0</v>
       </c>
-      <c r="H152" s="1">
+      <c r="H152">
         <v>25</v>
       </c>
       <c r="I152" s="1" t="s">
@@ -4813,7 +4813,7 @@
       <c r="G153" s="1">
         <v>0</v>
       </c>
-      <c r="H153" s="1">
+      <c r="H153">
         <v>89</v>
       </c>
       <c r="I153" s="1" t="s">
@@ -4842,7 +4842,7 @@
       <c r="G154" s="1">
         <v>0</v>
       </c>
-      <c r="H154" s="1">
+      <c r="H154">
         <v>52</v>
       </c>
       <c r="I154" s="1" t="s">
@@ -4871,7 +4871,7 @@
       <c r="G155" s="1">
         <v>0</v>
       </c>
-      <c r="H155" s="1">
+      <c r="H155">
         <v>33</v>
       </c>
       <c r="I155" s="1" t="s">
@@ -4900,7 +4900,7 @@
       <c r="G156" s="1">
         <v>0</v>
       </c>
-      <c r="H156" s="1">
+      <c r="H156">
         <v>37</v>
       </c>
       <c r="I156" s="1" t="s">
@@ -4929,7 +4929,7 @@
       <c r="G157" s="1">
         <v>0</v>
       </c>
-      <c r="H157" s="1">
+      <c r="H157">
         <v>37</v>
       </c>
       <c r="I157" s="1" t="s">
@@ -4958,7 +4958,7 @@
       <c r="G158" s="1">
         <v>0</v>
       </c>
-      <c r="H158" s="1">
+      <c r="H158">
         <v>26</v>
       </c>
       <c r="I158" s="1" t="s">
@@ -4987,7 +4987,7 @@
       <c r="G159" s="1">
         <v>0</v>
       </c>
-      <c r="H159" s="1">
+      <c r="H159">
         <v>41</v>
       </c>
       <c r="I159" s="1" t="s">
@@ -5016,7 +5016,7 @@
       <c r="G160" s="1">
         <v>0</v>
       </c>
-      <c r="H160" s="1">
+      <c r="H160">
         <v>64</v>
       </c>
       <c r="I160" s="1" t="s">
@@ -5045,7 +5045,7 @@
       <c r="G161" s="1">
         <v>0</v>
       </c>
-      <c r="H161" s="1">
+      <c r="H161">
         <v>55</v>
       </c>
       <c r="I161" s="1" t="s">
@@ -5074,7 +5074,7 @@
       <c r="G162" s="1">
         <v>0</v>
       </c>
-      <c r="H162" s="1">
+      <c r="H162">
         <v>77</v>
       </c>
       <c r="I162" s="1" t="s">
@@ -5103,7 +5103,7 @@
       <c r="G163" s="1">
         <v>0</v>
       </c>
-      <c r="H163" s="1">
+      <c r="H163">
         <v>70</v>
       </c>
       <c r="I163" s="1" t="s">
@@ -5132,7 +5132,7 @@
       <c r="G164" s="1">
         <v>0</v>
       </c>
-      <c r="H164" s="1">
+      <c r="H164">
         <v>68</v>
       </c>
       <c r="I164" s="1" t="s">
@@ -5161,7 +5161,7 @@
       <c r="G165" s="1">
         <v>0</v>
       </c>
-      <c r="H165" s="1">
+      <c r="H165">
         <v>93</v>
       </c>
       <c r="I165" s="1" t="s">
@@ -5190,7 +5190,7 @@
       <c r="G166" s="1">
         <v>0</v>
       </c>
-      <c r="H166" s="1">
+      <c r="H166">
         <v>98</v>
       </c>
       <c r="I166" s="1" t="s">
@@ -5219,7 +5219,7 @@
       <c r="G167" s="1">
         <v>0</v>
       </c>
-      <c r="H167" s="1">
+      <c r="H167">
         <v>55</v>
       </c>
       <c r="I167" s="1" t="s">
@@ -5248,7 +5248,7 @@
       <c r="G168" s="1">
         <v>0</v>
       </c>
-      <c r="H168" s="1">
+      <c r="H168">
         <v>15</v>
       </c>
       <c r="I168" s="1" t="s">
@@ -5277,7 +5277,7 @@
       <c r="G169" s="1">
         <v>0</v>
       </c>
-      <c r="H169" s="1">
+      <c r="H169">
         <v>10</v>
       </c>
       <c r="I169" s="1" t="s">
@@ -5306,7 +5306,7 @@
       <c r="G170" s="1">
         <v>0</v>
       </c>
-      <c r="H170" s="1">
+      <c r="H170">
         <v>60</v>
       </c>
       <c r="I170" s="1" t="s">
@@ -5335,7 +5335,7 @@
       <c r="G171" s="1">
         <v>0</v>
       </c>
-      <c r="H171" s="1">
+      <c r="H171">
         <v>96</v>
       </c>
       <c r="I171" s="1" t="s">
@@ -5364,7 +5364,7 @@
       <c r="G172" s="1">
         <v>0</v>
       </c>
-      <c r="H172" s="1">
+      <c r="H172">
         <v>42</v>
       </c>
       <c r="I172" s="1" t="s">
@@ -5393,7 +5393,7 @@
       <c r="G173" s="1">
         <v>0</v>
       </c>
-      <c r="H173" s="1">
+      <c r="H173">
         <v>54</v>
       </c>
       <c r="I173" s="1" t="s">
@@ -5422,7 +5422,7 @@
       <c r="G174" s="1">
         <v>0</v>
       </c>
-      <c r="H174" s="1">
+      <c r="H174">
         <v>86</v>
       </c>
       <c r="I174" s="1" t="s">
@@ -5451,7 +5451,7 @@
       <c r="G175" s="1">
         <v>0</v>
       </c>
-      <c r="H175" s="1">
+      <c r="H175">
         <v>91</v>
       </c>
       <c r="I175" s="1" t="s">
@@ -5480,7 +5480,7 @@
       <c r="G176" s="1">
         <v>0</v>
       </c>
-      <c r="H176" s="1">
+      <c r="H176">
         <v>19</v>
       </c>
       <c r="I176" s="1" t="s">
@@ -5509,7 +5509,7 @@
       <c r="G177" s="1">
         <v>0</v>
       </c>
-      <c r="H177" s="1">
+      <c r="H177">
         <v>52</v>
       </c>
       <c r="I177" s="1" t="s">
@@ -5538,7 +5538,7 @@
       <c r="G178" s="1">
         <v>0</v>
       </c>
-      <c r="H178" s="1">
+      <c r="H178">
         <v>29</v>
       </c>
       <c r="I178" s="1" t="s">
@@ -5567,7 +5567,7 @@
       <c r="G179" s="1">
         <v>0</v>
       </c>
-      <c r="H179" s="1">
+      <c r="H179">
         <v>50</v>
       </c>
       <c r="I179" s="1" t="s">
@@ -5596,7 +5596,7 @@
       <c r="G180" s="1">
         <v>0</v>
       </c>
-      <c r="H180" s="1">
+      <c r="H180">
         <v>13</v>
       </c>
       <c r="I180" s="1" t="s">
@@ -5625,7 +5625,7 @@
       <c r="G181" s="1">
         <v>0</v>
       </c>
-      <c r="H181" s="1">
+      <c r="H181">
         <v>85</v>
       </c>
       <c r="I181" s="1" t="s">
@@ -5654,7 +5654,7 @@
       <c r="G182" s="1">
         <v>0</v>
       </c>
-      <c r="H182" s="1">
+      <c r="H182">
         <v>32</v>
       </c>
       <c r="I182" s="1" t="s">
@@ -5683,8 +5683,8 @@
       <c r="G183" s="1">
         <v>0</v>
       </c>
-      <c r="H183" s="1">
-        <v>1</v>
+      <c r="H183">
+        <v>19</v>
       </c>
       <c r="I183" s="1" t="s">
         <v>6</v>
@@ -5712,7 +5712,7 @@
       <c r="G184" s="1">
         <v>0</v>
       </c>
-      <c r="H184" s="1">
+      <c r="H184">
         <v>68</v>
       </c>
       <c r="I184" s="1" t="s">
@@ -5741,7 +5741,7 @@
       <c r="G185" s="1">
         <v>0</v>
       </c>
-      <c r="H185" s="1">
+      <c r="H185">
         <v>73</v>
       </c>
       <c r="I185" s="1" t="s">
@@ -5770,7 +5770,7 @@
       <c r="G186" s="1">
         <v>0</v>
       </c>
-      <c r="H186" s="1">
+      <c r="H186">
         <v>48</v>
       </c>
       <c r="I186" s="1" t="s">
@@ -5799,7 +5799,7 @@
       <c r="G187" s="1">
         <v>0</v>
       </c>
-      <c r="H187" s="1">
+      <c r="H187">
         <v>30</v>
       </c>
       <c r="I187" s="1" t="s">
@@ -5828,7 +5828,7 @@
       <c r="G188" s="1">
         <v>0</v>
       </c>
-      <c r="H188" s="1">
+      <c r="H188">
         <v>85</v>
       </c>
       <c r="I188" s="1" t="s">
@@ -5857,7 +5857,7 @@
       <c r="G189" s="1">
         <v>0</v>
       </c>
-      <c r="H189" s="1">
+      <c r="H189">
         <v>68</v>
       </c>
       <c r="I189" s="1" t="s">
@@ -5886,7 +5886,7 @@
       <c r="G190" s="1">
         <v>0</v>
       </c>
-      <c r="H190" s="1">
+      <c r="H190">
         <v>25</v>
       </c>
       <c r="I190" s="1" t="s">
@@ -5915,7 +5915,7 @@
       <c r="G191" s="1">
         <v>0</v>
       </c>
-      <c r="H191" s="1">
+      <c r="H191">
         <v>54</v>
       </c>
       <c r="I191" s="1" t="s">
@@ -5944,7 +5944,7 @@
       <c r="G192" s="1">
         <v>0</v>
       </c>
-      <c r="H192" s="1">
+      <c r="H192">
         <v>75</v>
       </c>
       <c r="I192" s="1" t="s">
@@ -5973,7 +5973,7 @@
       <c r="G193" s="1">
         <v>0</v>
       </c>
-      <c r="H193" s="1">
+      <c r="H193">
         <v>32</v>
       </c>
       <c r="I193" s="1" t="s">
@@ -6002,7 +6002,7 @@
       <c r="G194" s="1">
         <v>0</v>
       </c>
-      <c r="H194" s="1">
+      <c r="H194">
         <v>47</v>
       </c>
       <c r="I194" s="1" t="s">
@@ -6031,7 +6031,7 @@
       <c r="G195" s="1">
         <v>0</v>
       </c>
-      <c r="H195" s="1">
+      <c r="H195">
         <v>90</v>
       </c>
       <c r="I195" s="1" t="s">
@@ -6060,7 +6060,7 @@
       <c r="G196" s="1">
         <v>0</v>
       </c>
-      <c r="H196" s="1">
+      <c r="H196">
         <v>11</v>
       </c>
       <c r="I196" s="1" t="s">
@@ -6089,7 +6089,7 @@
       <c r="G197" s="1">
         <v>0</v>
       </c>
-      <c r="H197" s="1">
+      <c r="H197">
         <v>87</v>
       </c>
       <c r="I197" s="1" t="s">
@@ -6118,7 +6118,7 @@
       <c r="G198" s="1">
         <v>0</v>
       </c>
-      <c r="H198" s="1">
+      <c r="H198">
         <v>78</v>
       </c>
       <c r="I198" s="1" t="s">
@@ -6147,7 +6147,7 @@
       <c r="G199" s="1">
         <v>0</v>
       </c>
-      <c r="H199" s="1">
+      <c r="H199">
         <v>13</v>
       </c>
       <c r="I199" s="1" t="s">
@@ -6176,7 +6176,7 @@
       <c r="G200" s="1">
         <v>0</v>
       </c>
-      <c r="H200" s="1">
+      <c r="H200">
         <v>97</v>
       </c>
       <c r="I200" s="1" t="s">
@@ -6205,7 +6205,7 @@
       <c r="G201" s="1">
         <v>0</v>
       </c>
-      <c r="H201" s="1">
+      <c r="H201">
         <v>26</v>
       </c>
       <c r="I201" s="1" t="s">
@@ -6234,7 +6234,7 @@
       <c r="G202" s="1">
         <v>0</v>
       </c>
-      <c r="H202" s="1">
+      <c r="H202">
         <v>22</v>
       </c>
       <c r="I202" s="1" t="s">
@@ -6263,7 +6263,7 @@
       <c r="G203" s="1">
         <v>0</v>
       </c>
-      <c r="H203" s="1">
+      <c r="H203">
         <v>22</v>
       </c>
       <c r="I203" s="1" t="s">
@@ -6292,7 +6292,7 @@
       <c r="G204" s="1">
         <v>0</v>
       </c>
-      <c r="H204" s="1">
+      <c r="H204">
         <v>66</v>
       </c>
       <c r="I204" s="1" t="s">
@@ -6321,7 +6321,7 @@
       <c r="G205" s="1">
         <v>0</v>
       </c>
-      <c r="H205" s="1">
+      <c r="H205">
         <v>45</v>
       </c>
       <c r="I205" s="1" t="s">
@@ -6350,7 +6350,7 @@
       <c r="G206" s="1">
         <v>0</v>
       </c>
-      <c r="H206" s="1">
+      <c r="H206">
         <v>95</v>
       </c>
       <c r="I206" s="1" t="s">
@@ -6379,7 +6379,7 @@
       <c r="G207" s="1">
         <v>0</v>
       </c>
-      <c r="H207" s="1">
+      <c r="H207">
         <v>61</v>
       </c>
       <c r="I207" s="1" t="s">
@@ -6408,7 +6408,7 @@
       <c r="G208" s="1">
         <v>0</v>
       </c>
-      <c r="H208" s="1">
+      <c r="H208">
         <v>96</v>
       </c>
       <c r="I208" s="1" t="s">
@@ -6437,7 +6437,7 @@
       <c r="G209" s="1">
         <v>0</v>
       </c>
-      <c r="H209" s="1">
+      <c r="H209">
         <v>83</v>
       </c>
       <c r="I209" s="1" t="s">
@@ -6466,7 +6466,7 @@
       <c r="G210" s="1">
         <v>0</v>
       </c>
-      <c r="H210" s="1">
+      <c r="H210">
         <v>89</v>
       </c>
       <c r="I210" s="1" t="s">
@@ -6495,7 +6495,7 @@
       <c r="G211" s="1">
         <v>0</v>
       </c>
-      <c r="H211" s="1">
+      <c r="H211">
         <v>82</v>
       </c>
       <c r="I211" s="1" t="s">
@@ -6524,7 +6524,7 @@
       <c r="G212" s="1">
         <v>0</v>
       </c>
-      <c r="H212" s="1">
+      <c r="H212">
         <v>23</v>
       </c>
       <c r="I212" s="1" t="s">
@@ -6553,7 +6553,7 @@
       <c r="G213" s="1">
         <v>0</v>
       </c>
-      <c r="H213" s="1">
+      <c r="H213">
         <v>46</v>
       </c>
       <c r="I213" s="1" t="s">
@@ -6582,7 +6582,7 @@
       <c r="G214" s="1">
         <v>0</v>
       </c>
-      <c r="H214" s="1">
+      <c r="H214">
         <v>87</v>
       </c>
       <c r="I214" s="1" t="s">
@@ -6611,7 +6611,7 @@
       <c r="G215" s="1">
         <v>0</v>
       </c>
-      <c r="H215" s="1">
+      <c r="H215">
         <v>35</v>
       </c>
       <c r="I215" s="1" t="s">
@@ -6640,7 +6640,7 @@
       <c r="G216" s="1">
         <v>0</v>
       </c>
-      <c r="H216" s="1">
+      <c r="H216">
         <v>91</v>
       </c>
       <c r="I216" s="1" t="s">
@@ -6669,8 +6669,8 @@
       <c r="G217" s="1">
         <v>0</v>
       </c>
-      <c r="H217" s="1">
-        <v>8</v>
+      <c r="H217">
+        <v>88</v>
       </c>
       <c r="I217" s="1" t="s">
         <v>6</v>
@@ -6698,7 +6698,7 @@
       <c r="G218" s="1">
         <v>0</v>
       </c>
-      <c r="H218" s="1">
+      <c r="H218">
         <v>57</v>
       </c>
       <c r="I218" s="1" t="s">
@@ -6727,8 +6727,8 @@
       <c r="G219" s="1">
         <v>0</v>
       </c>
-      <c r="H219" s="1">
-        <v>5</v>
+      <c r="H219">
+        <v>52</v>
       </c>
       <c r="I219" s="1" t="s">
         <v>6</v>
@@ -6756,7 +6756,7 @@
       <c r="G220" s="1">
         <v>0</v>
       </c>
-      <c r="H220" s="1">
+      <c r="H220">
         <v>70</v>
       </c>
       <c r="I220" s="1" t="s">
@@ -6785,7 +6785,7 @@
       <c r="G221" s="1">
         <v>0</v>
       </c>
-      <c r="H221" s="1">
+      <c r="H221">
         <v>88</v>
       </c>
       <c r="I221" s="1" t="s">
@@ -6814,7 +6814,7 @@
       <c r="G222" s="1">
         <v>0</v>
       </c>
-      <c r="H222" s="1">
+      <c r="H222">
         <v>22</v>
       </c>
       <c r="I222" s="1" t="s">
@@ -6843,7 +6843,7 @@
       <c r="G223" s="1">
         <v>0</v>
       </c>
-      <c r="H223" s="1">
+      <c r="H223">
         <v>62</v>
       </c>
       <c r="I223" s="1" t="s">
@@ -6872,7 +6872,7 @@
       <c r="G224" s="1">
         <v>0</v>
       </c>
-      <c r="H224" s="1">
+      <c r="H224">
         <v>12</v>
       </c>
       <c r="I224" s="1" t="s">
@@ -6901,8 +6901,8 @@
       <c r="G225" s="1">
         <v>0</v>
       </c>
-      <c r="H225" s="1">
-        <v>7</v>
+      <c r="H225">
+        <v>75</v>
       </c>
       <c r="I225" s="1" t="s">
         <v>6</v>
@@ -6930,7 +6930,7 @@
       <c r="G226" s="1">
         <v>0</v>
       </c>
-      <c r="H226" s="1">
+      <c r="H226">
         <v>81</v>
       </c>
       <c r="I226" s="1" t="s">
@@ -6959,7 +6959,7 @@
       <c r="G227" s="1">
         <v>0</v>
       </c>
-      <c r="H227" s="1">
+      <c r="H227">
         <v>32</v>
       </c>
       <c r="I227" s="1" t="s">
@@ -6988,7 +6988,7 @@
       <c r="G228" s="1">
         <v>0</v>
       </c>
-      <c r="H228" s="1">
+      <c r="H228">
         <v>84</v>
       </c>
       <c r="I228" s="1" t="s">
@@ -7017,7 +7017,7 @@
       <c r="G229" s="1">
         <v>0</v>
       </c>
-      <c r="H229" s="1">
+      <c r="H229">
         <v>17</v>
       </c>
       <c r="I229" s="1" t="s">
@@ -7046,8 +7046,8 @@
       <c r="G230" s="1">
         <v>0</v>
       </c>
-      <c r="H230" s="1">
-        <v>7</v>
+      <c r="H230">
+        <v>29</v>
       </c>
       <c r="I230" s="1" t="s">
         <v>6</v>
@@ -7075,7 +7075,7 @@
       <c r="G231" s="1">
         <v>0</v>
       </c>
-      <c r="H231" s="1">
+      <c r="H231">
         <v>79</v>
       </c>
       <c r="I231" s="1" t="s">
@@ -7104,7 +7104,7 @@
       <c r="G232" s="1">
         <v>0</v>
       </c>
-      <c r="H232" s="1">
+      <c r="H232">
         <v>46</v>
       </c>
       <c r="I232" s="1" t="s">
@@ -7133,8 +7133,8 @@
       <c r="G233" s="1">
         <v>0</v>
       </c>
-      <c r="H233" s="1">
-        <v>2</v>
+      <c r="H233">
+        <v>52</v>
       </c>
       <c r="I233" s="1" t="s">
         <v>6</v>
@@ -7162,8 +7162,8 @@
       <c r="G234" s="1">
         <v>0</v>
       </c>
-      <c r="H234" s="1">
-        <v>6</v>
+      <c r="H234">
+        <v>81</v>
       </c>
       <c r="I234" s="1" t="s">
         <v>6</v>
@@ -7191,8 +7191,8 @@
       <c r="G235" s="1">
         <v>0</v>
       </c>
-      <c r="H235" s="1">
-        <v>0</v>
+      <c r="H235">
+        <v>60</v>
       </c>
       <c r="I235" s="1" t="s">
         <v>6</v>
@@ -7220,8 +7220,8 @@
       <c r="G236" s="1">
         <v>0</v>
       </c>
-      <c r="H236" s="1">
-        <v>2</v>
+      <c r="H236">
+        <v>27</v>
       </c>
       <c r="I236" s="1" t="s">
         <v>6</v>
@@ -7249,7 +7249,7 @@
       <c r="G237" s="1">
         <v>0</v>
       </c>
-      <c r="H237" s="1">
+      <c r="H237">
         <v>19</v>
       </c>
       <c r="I237" s="1" t="s">
@@ -7278,7 +7278,7 @@
       <c r="G238" s="1">
         <v>0</v>
       </c>
-      <c r="H238" s="1">
+      <c r="H238">
         <v>99</v>
       </c>
       <c r="I238" s="1" t="s">
@@ -7307,7 +7307,7 @@
       <c r="G239" s="1">
         <v>0</v>
       </c>
-      <c r="H239" s="1">
+      <c r="H239">
         <v>58</v>
       </c>
       <c r="I239" s="1" t="s">
@@ -7336,7 +7336,7 @@
       <c r="G240" s="1">
         <v>0</v>
       </c>
-      <c r="H240" s="1">
+      <c r="H240">
         <v>34</v>
       </c>
       <c r="I240" s="1" t="s">
@@ -7365,7 +7365,7 @@
       <c r="G241" s="1">
         <v>0</v>
       </c>
-      <c r="H241" s="1">
+      <c r="H241">
         <v>97</v>
       </c>
       <c r="I241" s="1" t="s">
@@ -7394,7 +7394,7 @@
       <c r="G242" s="1">
         <v>0</v>
       </c>
-      <c r="H242" s="1">
+      <c r="H242">
         <v>97</v>
       </c>
       <c r="I242" s="1" t="s">
@@ -7423,7 +7423,7 @@
       <c r="G243" s="1">
         <v>0</v>
       </c>
-      <c r="H243" s="1">
+      <c r="H243">
         <v>11</v>
       </c>
       <c r="I243" s="1" t="s">
@@ -7452,7 +7452,7 @@
       <c r="G244" s="1">
         <v>0</v>
       </c>
-      <c r="H244" s="1">
+      <c r="H244">
         <v>22</v>
       </c>
       <c r="I244" s="1" t="s">
@@ -7481,7 +7481,7 @@
       <c r="G245" s="1">
         <v>0</v>
       </c>
-      <c r="H245" s="1">
+      <c r="H245">
         <v>88</v>
       </c>
       <c r="I245" s="1" t="s">
@@ -7510,7 +7510,7 @@
       <c r="G246" s="1">
         <v>0</v>
       </c>
-      <c r="H246" s="1">
+      <c r="H246">
         <v>83</v>
       </c>
       <c r="I246" s="1" t="s">
@@ -7539,7 +7539,7 @@
       <c r="G247" s="1">
         <v>0</v>
       </c>
-      <c r="H247" s="1">
+      <c r="H247">
         <v>88</v>
       </c>
       <c r="I247" s="1" t="s">
@@ -7568,7 +7568,7 @@
       <c r="G248" s="1">
         <v>0</v>
       </c>
-      <c r="H248" s="1">
+      <c r="H248">
         <v>46</v>
       </c>
       <c r="I248" s="1" t="s">
@@ -7597,7 +7597,7 @@
       <c r="G249" s="1">
         <v>0</v>
       </c>
-      <c r="H249" s="1">
+      <c r="H249">
         <v>63</v>
       </c>
       <c r="I249" s="1" t="s">
@@ -7626,7 +7626,7 @@
       <c r="G250" s="1">
         <v>0</v>
       </c>
-      <c r="H250" s="1">
+      <c r="H250">
         <v>40</v>
       </c>
       <c r="I250" s="1" t="s">
@@ -7655,7 +7655,7 @@
       <c r="G251" s="1">
         <v>0</v>
       </c>
-      <c r="H251" s="1">
+      <c r="H251">
         <v>79</v>
       </c>
       <c r="I251" s="1" t="s">
@@ -7684,7 +7684,7 @@
       <c r="G252" s="1">
         <v>0</v>
       </c>
-      <c r="H252" s="1">
+      <c r="H252">
         <v>67</v>
       </c>
       <c r="I252" s="1" t="s">
@@ -7713,7 +7713,7 @@
       <c r="G253" s="1">
         <v>0</v>
       </c>
-      <c r="H253" s="1">
+      <c r="H253">
         <v>39</v>
       </c>
       <c r="I253" s="1" t="s">
@@ -7742,8 +7742,8 @@
       <c r="G254" s="1">
         <v>0</v>
       </c>
-      <c r="H254" s="1">
-        <v>9</v>
+      <c r="H254">
+        <v>63</v>
       </c>
       <c r="I254" s="1" t="s">
         <v>6</v>
@@ -7771,7 +7771,7 @@
       <c r="G255" s="1">
         <v>0</v>
       </c>
-      <c r="H255" s="1">
+      <c r="H255">
         <v>25</v>
       </c>
       <c r="I255" s="1" t="s">
@@ -7800,7 +7800,7 @@
       <c r="G256" s="1">
         <v>0</v>
       </c>
-      <c r="H256" s="1">
+      <c r="H256">
         <v>31</v>
       </c>
       <c r="I256" s="1" t="s">
@@ -7829,7 +7829,7 @@
       <c r="G257" s="1">
         <v>0</v>
       </c>
-      <c r="H257" s="1">
+      <c r="H257">
         <v>33</v>
       </c>
       <c r="I257" s="1" t="s">
@@ -7858,7 +7858,7 @@
       <c r="G258" s="1">
         <v>0</v>
       </c>
-      <c r="H258" s="1">
+      <c r="H258">
         <v>24</v>
       </c>
       <c r="I258" s="1" t="s">
@@ -7887,7 +7887,7 @@
       <c r="G259" s="1">
         <v>0</v>
       </c>
-      <c r="H259" s="1">
+      <c r="H259">
         <v>39</v>
       </c>
       <c r="I259" s="1" t="s">
@@ -7916,7 +7916,7 @@
       <c r="G260" s="1">
         <v>0</v>
       </c>
-      <c r="H260" s="1">
+      <c r="H260">
         <v>10</v>
       </c>
       <c r="I260" s="1" t="s">
@@ -7945,7 +7945,7 @@
       <c r="G261" s="1">
         <v>0</v>
       </c>
-      <c r="H261" s="1">
+      <c r="H261">
         <v>17</v>
       </c>
       <c r="I261" s="1" t="s">
@@ -7974,7 +7974,7 @@
       <c r="G262" s="1">
         <v>0</v>
       </c>
-      <c r="H262" s="1">
+      <c r="H262">
         <v>76</v>
       </c>
       <c r="I262" s="1" t="s">
@@ -8003,7 +8003,7 @@
       <c r="G263" s="1">
         <v>0</v>
       </c>
-      <c r="H263" s="1">
+      <c r="H263">
         <v>86</v>
       </c>
       <c r="I263" s="1" t="s">
@@ -8032,7 +8032,7 @@
       <c r="G264" s="1">
         <v>0</v>
       </c>
-      <c r="H264" s="1">
+      <c r="H264">
         <v>29</v>
       </c>
       <c r="I264" s="1" t="s">
@@ -8061,7 +8061,7 @@
       <c r="G265" s="1">
         <v>0</v>
       </c>
-      <c r="H265" s="1">
+      <c r="H265">
         <v>52</v>
       </c>
       <c r="I265" s="1" t="s">
@@ -8090,7 +8090,7 @@
       <c r="G266" s="1">
         <v>0</v>
       </c>
-      <c r="H266" s="1">
+      <c r="H266">
         <v>91</v>
       </c>
       <c r="I266" s="1" t="s">
@@ -8119,7 +8119,7 @@
       <c r="G267" s="1">
         <v>0</v>
       </c>
-      <c r="H267" s="1">
+      <c r="H267">
         <v>79</v>
       </c>
       <c r="I267" s="1" t="s">
@@ -8148,7 +8148,7 @@
       <c r="G268" s="1">
         <v>0</v>
       </c>
-      <c r="H268" s="1">
+      <c r="H268">
         <v>99</v>
       </c>
       <c r="I268" s="1" t="s">
@@ -8177,7 +8177,7 @@
       <c r="G269" s="1">
         <v>0</v>
       </c>
-      <c r="H269" s="1">
+      <c r="H269">
         <v>54</v>
       </c>
       <c r="I269" s="1" t="s">
@@ -8206,8 +8206,8 @@
       <c r="G270" s="1">
         <v>0</v>
       </c>
-      <c r="H270" s="1">
-        <v>3</v>
+      <c r="H270">
+        <v>32</v>
       </c>
       <c r="I270" s="1" t="s">
         <v>6</v>
@@ -8235,7 +8235,7 @@
       <c r="G271" s="1">
         <v>0</v>
       </c>
-      <c r="H271" s="1">
+      <c r="H271">
         <v>60</v>
       </c>
       <c r="I271" s="1" t="s">
@@ -8264,7 +8264,7 @@
       <c r="G272" s="1">
         <v>0</v>
       </c>
-      <c r="H272" s="1">
+      <c r="H272">
         <v>69</v>
       </c>
       <c r="I272" s="1" t="s">
@@ -8293,7 +8293,7 @@
       <c r="G273" s="1">
         <v>0</v>
       </c>
-      <c r="H273" s="1">
+      <c r="H273">
         <v>95</v>
       </c>
       <c r="I273" s="1" t="s">
@@ -8322,7 +8322,7 @@
       <c r="G274" s="1">
         <v>0</v>
       </c>
-      <c r="H274" s="1">
+      <c r="H274">
         <v>57</v>
       </c>
       <c r="I274" s="1" t="s">
@@ -8351,7 +8351,7 @@
       <c r="G275" s="1">
         <v>0</v>
       </c>
-      <c r="H275" s="1">
+      <c r="H275">
         <v>43</v>
       </c>
       <c r="I275" s="1" t="s">
@@ -8380,7 +8380,7 @@
       <c r="G276" s="1">
         <v>0</v>
       </c>
-      <c r="H276" s="1">
+      <c r="H276">
         <v>89</v>
       </c>
       <c r="I276" s="1" t="s">
@@ -8409,7 +8409,7 @@
       <c r="G277" s="1">
         <v>0</v>
       </c>
-      <c r="H277" s="1">
+      <c r="H277">
         <v>77</v>
       </c>
       <c r="I277" s="1" t="s">
@@ -8438,7 +8438,7 @@
       <c r="G278" s="1">
         <v>0</v>
       </c>
-      <c r="H278" s="1">
+      <c r="H278">
         <v>28</v>
       </c>
       <c r="I278" s="1" t="s">
@@ -8467,7 +8467,7 @@
       <c r="G279" s="1">
         <v>0</v>
       </c>
-      <c r="H279" s="1">
+      <c r="H279">
         <v>53</v>
       </c>
       <c r="I279" s="1" t="s">
@@ -8496,7 +8496,7 @@
       <c r="G280" s="1">
         <v>0</v>
       </c>
-      <c r="H280" s="1">
+      <c r="H280">
         <v>79</v>
       </c>
       <c r="I280" s="1" t="s">
@@ -8525,7 +8525,7 @@
       <c r="G281" s="1">
         <v>0</v>
       </c>
-      <c r="H281" s="1">
+      <c r="H281">
         <v>80</v>
       </c>
       <c r="I281" s="1" t="s">
@@ -8554,7 +8554,7 @@
       <c r="G282" s="1">
         <v>0</v>
       </c>
-      <c r="H282" s="1">
+      <c r="H282">
         <v>66</v>
       </c>
       <c r="I282" s="1" t="s">
@@ -8583,7 +8583,7 @@
       <c r="G283" s="1">
         <v>0</v>
       </c>
-      <c r="H283" s="1">
+      <c r="H283">
         <v>76</v>
       </c>
       <c r="I283" s="1" t="s">
@@ -8612,7 +8612,7 @@
       <c r="G284" s="1">
         <v>0</v>
       </c>
-      <c r="H284" s="1">
+      <c r="H284">
         <v>64</v>
       </c>
       <c r="I284" s="1" t="s">
@@ -8641,7 +8641,7 @@
       <c r="G285" s="1">
         <v>0</v>
       </c>
-      <c r="H285" s="1">
+      <c r="H285">
         <v>42</v>
       </c>
       <c r="I285" s="1" t="s">
@@ -8670,7 +8670,7 @@
       <c r="G286" s="1">
         <v>0</v>
       </c>
-      <c r="H286" s="1">
+      <c r="H286">
         <v>49</v>
       </c>
       <c r="I286" s="1" t="s">
@@ -8699,7 +8699,7 @@
       <c r="G287" s="1">
         <v>0</v>
       </c>
-      <c r="H287" s="1">
+      <c r="H287">
         <v>46</v>
       </c>
       <c r="I287" s="1" t="s">
@@ -8728,7 +8728,7 @@
       <c r="G288" s="1">
         <v>0</v>
       </c>
-      <c r="H288" s="1">
+      <c r="H288">
         <v>28</v>
       </c>
       <c r="I288" s="1" t="s">
@@ -8757,7 +8757,7 @@
       <c r="G289" s="1">
         <v>0</v>
       </c>
-      <c r="H289" s="1">
+      <c r="H289">
         <v>43</v>
       </c>
       <c r="I289" s="1" t="s">
@@ -8786,8 +8786,8 @@
       <c r="G290" s="1">
         <v>0</v>
       </c>
-      <c r="H290" s="1">
-        <v>8</v>
+      <c r="H290">
+        <v>80</v>
       </c>
       <c r="I290" s="1" t="s">
         <v>6</v>
@@ -8815,7 +8815,7 @@
       <c r="G291" s="1">
         <v>0</v>
       </c>
-      <c r="H291" s="1">
+      <c r="H291">
         <v>96</v>
       </c>
       <c r="I291" s="1" t="s">
@@ -8844,7 +8844,7 @@
       <c r="G292" s="1">
         <v>0</v>
       </c>
-      <c r="H292" s="1">
+      <c r="H292">
         <v>74</v>
       </c>
       <c r="I292" s="1" t="s">
@@ -8873,7 +8873,7 @@
       <c r="G293" s="1">
         <v>0</v>
       </c>
-      <c r="H293" s="1">
+      <c r="H293">
         <v>62</v>
       </c>
       <c r="I293" s="1" t="s">
@@ -8902,7 +8902,7 @@
       <c r="G294" s="1">
         <v>0</v>
       </c>
-      <c r="H294" s="1">
+      <c r="H294">
         <v>60</v>
       </c>
       <c r="I294" s="1" t="s">
@@ -8931,7 +8931,7 @@
       <c r="G295" s="1">
         <v>0</v>
       </c>
-      <c r="H295" s="1">
+      <c r="H295">
         <v>21</v>
       </c>
       <c r="I295" s="1" t="s">
@@ -8960,7 +8960,7 @@
       <c r="G296" s="1">
         <v>0</v>
       </c>
-      <c r="H296" s="1">
+      <c r="H296">
         <v>99</v>
       </c>
       <c r="I296" s="1" t="s">
@@ -8989,8 +8989,8 @@
       <c r="G297" s="1">
         <v>0</v>
       </c>
-      <c r="H297" s="1">
-        <v>5</v>
+      <c r="H297">
+        <v>56</v>
       </c>
       <c r="I297" s="1" t="s">
         <v>6</v>
@@ -9018,7 +9018,7 @@
       <c r="G298" s="1">
         <v>0</v>
       </c>
-      <c r="H298" s="1">
+      <c r="H298">
         <v>10</v>
       </c>
       <c r="I298" s="1" t="s">
@@ -9047,7 +9047,7 @@
       <c r="G299" s="1">
         <v>0</v>
       </c>
-      <c r="H299" s="1">
+      <c r="H299">
         <v>66</v>
       </c>
       <c r="I299" s="1" t="s">
@@ -9076,7 +9076,7 @@
       <c r="G300" s="1">
         <v>0</v>
       </c>
-      <c r="H300" s="1">
+      <c r="H300">
         <v>84</v>
       </c>
       <c r="I300" s="1" t="s">
@@ -9105,7 +9105,7 @@
       <c r="G301" s="1">
         <v>0</v>
       </c>
-      <c r="H301" s="1">
+      <c r="H301">
         <v>58</v>
       </c>
       <c r="I301" s="1" t="s">
@@ -9134,7 +9134,7 @@
       <c r="G302" s="1">
         <v>0</v>
       </c>
-      <c r="H302" s="1">
+      <c r="H302">
         <v>44</v>
       </c>
       <c r="I302" s="1" t="s">
@@ -9163,7 +9163,7 @@
       <c r="G303" s="1">
         <v>0</v>
       </c>
-      <c r="H303" s="1">
+      <c r="H303">
         <v>75</v>
       </c>
       <c r="I303" s="1" t="s">
@@ -9192,7 +9192,7 @@
       <c r="G304" s="1">
         <v>0</v>
       </c>
-      <c r="H304" s="1">
+      <c r="H304">
         <v>34</v>
       </c>
       <c r="I304" s="1" t="s">
@@ -9221,7 +9221,7 @@
       <c r="G305" s="1">
         <v>0</v>
       </c>
-      <c r="H305" s="1">
+      <c r="H305">
         <v>81</v>
       </c>
       <c r="I305" s="1" t="s">
@@ -9250,7 +9250,7 @@
       <c r="G306" s="1">
         <v>0</v>
       </c>
-      <c r="H306" s="1">
+      <c r="H306">
         <v>22</v>
       </c>
       <c r="I306" s="1" t="s">
@@ -9279,7 +9279,7 @@
       <c r="G307" s="1">
         <v>0</v>
       </c>
-      <c r="H307" s="1">
+      <c r="H307">
         <v>36</v>
       </c>
       <c r="I307" s="1" t="s">
@@ -9308,7 +9308,7 @@
       <c r="G308" s="1">
         <v>0</v>
       </c>
-      <c r="H308" s="1">
+      <c r="H308">
         <v>19</v>
       </c>
       <c r="I308" s="1" t="s">
@@ -9337,7 +9337,7 @@
       <c r="G309" s="1">
         <v>0</v>
       </c>
-      <c r="H309" s="1">
+      <c r="H309">
         <v>21</v>
       </c>
       <c r="I309" s="1" t="s">
@@ -9366,7 +9366,7 @@
       <c r="G310" s="1">
         <v>0</v>
       </c>
-      <c r="H310" s="1">
+      <c r="H310">
         <v>51</v>
       </c>
       <c r="I310" s="1" t="s">
@@ -9395,7 +9395,7 @@
       <c r="G311" s="1">
         <v>0</v>
       </c>
-      <c r="H311" s="1">
+      <c r="H311">
         <v>45</v>
       </c>
       <c r="I311" s="1" t="s">
@@ -9424,7 +9424,7 @@
       <c r="G312" s="1">
         <v>0</v>
       </c>
-      <c r="H312" s="1">
+      <c r="H312">
         <v>76</v>
       </c>
       <c r="I312" s="1" t="s">
@@ -9453,7 +9453,7 @@
       <c r="G313" s="1">
         <v>0</v>
       </c>
-      <c r="H313" s="1">
+      <c r="H313">
         <v>86</v>
       </c>
       <c r="I313" s="1" t="s">
@@ -9482,8 +9482,8 @@
       <c r="G314" s="1">
         <v>0</v>
       </c>
-      <c r="H314" s="1">
-        <v>6</v>
+      <c r="H314">
+        <v>40</v>
       </c>
       <c r="I314" s="1" t="s">
         <v>6</v>
@@ -9511,7 +9511,7 @@
       <c r="G315" s="1">
         <v>0</v>
       </c>
-      <c r="H315" s="1">
+      <c r="H315">
         <v>76</v>
       </c>
       <c r="I315" s="1" t="s">
@@ -9540,7 +9540,7 @@
       <c r="G316" s="1">
         <v>0</v>
       </c>
-      <c r="H316" s="1">
+      <c r="H316">
         <v>37</v>
       </c>
       <c r="I316" s="1" t="s">
@@ -9569,7 +9569,7 @@
       <c r="G317" s="1">
         <v>0</v>
       </c>
-      <c r="H317" s="1">
+      <c r="H317">
         <v>23</v>
       </c>
       <c r="I317" s="1" t="s">
@@ -9598,7 +9598,7 @@
       <c r="G318" s="1">
         <v>0</v>
       </c>
-      <c r="H318" s="1">
+      <c r="H318">
         <v>75</v>
       </c>
       <c r="I318" s="1" t="s">
@@ -9627,7 +9627,7 @@
       <c r="G319" s="1">
         <v>0</v>
       </c>
-      <c r="H319" s="1">
+      <c r="H319">
         <v>44</v>
       </c>
       <c r="I319" s="1" t="s">
@@ -9656,7 +9656,7 @@
       <c r="G320" s="1">
         <v>0</v>
       </c>
-      <c r="H320" s="1">
+      <c r="H320">
         <v>60</v>
       </c>
       <c r="I320" s="1" t="s">
@@ -9685,7 +9685,7 @@
       <c r="G321" s="1">
         <v>0</v>
       </c>
-      <c r="H321" s="1">
+      <c r="H321">
         <v>54</v>
       </c>
       <c r="I321" s="1" t="s">
@@ -9714,7 +9714,7 @@
       <c r="G322" s="1">
         <v>0</v>
       </c>
-      <c r="H322" s="1">
+      <c r="H322">
         <v>99</v>
       </c>
       <c r="I322" s="1" t="s">
@@ -9743,8 +9743,8 @@
       <c r="G323" s="1">
         <v>0</v>
       </c>
-      <c r="H323" s="1">
-        <v>9</v>
+      <c r="H323">
+        <v>82</v>
       </c>
       <c r="I323" s="1" t="s">
         <v>6</v>
@@ -9772,7 +9772,7 @@
       <c r="G324" s="1">
         <v>0</v>
       </c>
-      <c r="H324" s="1">
+      <c r="H324">
         <v>77</v>
       </c>
       <c r="I324" s="1" t="s">
@@ -9801,7 +9801,7 @@
       <c r="G325" s="1">
         <v>0</v>
       </c>
-      <c r="H325" s="1">
+      <c r="H325">
         <v>81</v>
       </c>
       <c r="I325" s="1" t="s">
@@ -9830,7 +9830,7 @@
       <c r="G326" s="1">
         <v>0</v>
       </c>
-      <c r="H326" s="1">
+      <c r="H326">
         <v>86</v>
       </c>
       <c r="I326" s="1" t="s">
@@ -9859,7 +9859,7 @@
       <c r="G327" s="1">
         <v>0</v>
       </c>
-      <c r="H327" s="1">
+      <c r="H327">
         <v>31</v>
       </c>
       <c r="I327" s="1" t="s">
@@ -9888,7 +9888,7 @@
       <c r="G328" s="1">
         <v>0</v>
       </c>
-      <c r="H328" s="1">
+      <c r="H328">
         <v>53</v>
       </c>
       <c r="I328" s="1" t="s">
@@ -9917,7 +9917,7 @@
       <c r="G329" s="1">
         <v>0</v>
       </c>
-      <c r="H329" s="1">
+      <c r="H329">
         <v>34</v>
       </c>
       <c r="I329" s="1" t="s">
@@ -9946,7 +9946,7 @@
       <c r="G330" s="1">
         <v>0</v>
       </c>
-      <c r="H330" s="1">
+      <c r="H330">
         <v>78</v>
       </c>
       <c r="I330" s="1" t="s">
@@ -9975,7 +9975,7 @@
       <c r="G331" s="1">
         <v>0</v>
       </c>
-      <c r="H331" s="1">
+      <c r="H331">
         <v>94</v>
       </c>
       <c r="I331" s="1" t="s">
@@ -10004,7 +10004,7 @@
       <c r="G332" s="1">
         <v>0</v>
       </c>
-      <c r="H332" s="1">
+      <c r="H332">
         <v>13</v>
       </c>
       <c r="I332" s="1" t="s">
@@ -10033,7 +10033,7 @@
       <c r="G333" s="1">
         <v>0</v>
       </c>
-      <c r="H333" s="1">
+      <c r="H333">
         <v>92</v>
       </c>
       <c r="I333" s="1" t="s">
@@ -10062,7 +10062,7 @@
       <c r="G334" s="1">
         <v>0</v>
       </c>
-      <c r="H334" s="1">
+      <c r="H334">
         <v>98</v>
       </c>
       <c r="I334" s="1" t="s">
@@ -10091,7 +10091,7 @@
       <c r="G335" s="1">
         <v>0</v>
       </c>
-      <c r="H335" s="1">
+      <c r="H335">
         <v>42</v>
       </c>
       <c r="I335" s="1" t="s">

</xml_diff>